<commit_message>
Finalizacion de actividad 2
</commit_message>
<xml_diff>
--- a/Concatenaciones.xlsx
+++ b/Concatenaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correobuap-my.sharepoint.com/personal/kevin_armas_alumno_buap_mx/Documents/School/7mo semestre/Modelos de desarrollo Web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77B5400-9A16-4FE0-9B8B-F9BAF7FC9CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D77B5400-9A16-4FE0-9B8B-F9BAF7FC9CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{824EF041-C554-4E77-B067-65995843A042}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{324761CA-E09D-4A73-9500-63BF426B3120}"/>
   </bookViews>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918AAC57-A6A0-4244-A2C7-328E32E4AA80}">
   <dimension ref="A1:E235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>